<commit_message>
Import To Github 4th time
</commit_message>
<xml_diff>
--- a/OutputData.xlsx
+++ b/OutputData.xlsx
@@ -65,7 +65,7 @@
     <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
   </si>
   <si>
-    <t>20 hours, 29 minutes</t>
+    <t>20 hours, 34 minutes</t>
   </si>
   <si>
     <t>1648789K</t>
@@ -788,10 +788,10 @@
         <v>1688360784</v>
       </c>
       <c r="C3" t="n">
-        <v>405609856</v>
+        <v>405610408</v>
       </c>
       <c r="D3" t="n">
-        <v>1282750928</v>
+        <v>1282750376</v>
       </c>
       <c r="E3">
         <f>IF(ISERROR(C3/B3),0,(C3/B3)*100)</f>
@@ -870,7 +870,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="n">
-        <v>313303</v>
+        <v>314690</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="n">
-        <v>302618</v>
+        <v>304127</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>68589</v>
+        <v>68852</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -939,7 +939,7 @@
         <v>58</v>
       </c>
       <c r="C5" t="n">
-        <v>44342</v>
+        <v>44516</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Import To Github 5th time
</commit_message>
<xml_diff>
--- a/OutputData.xlsx
+++ b/OutputData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Hostname</t>
   </si>
@@ -65,7 +65,7 @@
     <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
   </si>
   <si>
-    <t>20 hours, 34 minutes</t>
+    <t>23 hours, 29 minutes</t>
   </si>
   <si>
     <t>1648789K</t>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>1%</t>
-  </si>
-  <si>
-    <t>0%</t>
   </si>
   <si>
     <t>Variable</t>
@@ -788,10 +785,10 @@
         <v>1688360784</v>
       </c>
       <c r="C3" t="n">
-        <v>405610408</v>
+        <v>405609916</v>
       </c>
       <c r="D3" t="n">
-        <v>1282750376</v>
+        <v>1282750868</v>
       </c>
       <c r="E3">
         <f>IF(ISERROR(C3/B3),0,(C3/B3)*100)</f>
@@ -808,7 +805,7 @@
         <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J3">
         <f>IF((VALUE(I3)*100)&lt;=40,"Excellent",IF((VALUE(I3)*100)&lt;=60,"Good",IF((VALUE(I3)*100)&lt;=80,"Fair","Poor")))</f>
@@ -844,19 +841,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>43</v>
@@ -867,10 +864,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="n">
-        <v>314690</v>
+        <v>357556</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -890,10 +887,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="n">
-        <v>304127</v>
+        <v>348792</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -913,10 +910,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="n">
-        <v>68852</v>
+        <v>78291</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -936,10 +933,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="n">
-        <v>44516</v>
+        <v>50819</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
@@ -959,7 +956,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
@@ -982,7 +979,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -1024,7 +1021,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1036,10 +1033,10 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import To Github 6th time
</commit_message>
<xml_diff>
--- a/OutputData.xlsx
+++ b/OutputData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Hostname</t>
   </si>
@@ -47,90 +47,111 @@
     <t>FLASH</t>
   </si>
   <si>
+    <t>VG-203</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ISR4331/K9        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4331 Chassis"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FDO2110A2LG</t>
+  </si>
+  <si>
+    <t>15.5(3)S4b</t>
+  </si>
+  <si>
+    <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
+  </si>
+  <si>
+    <t>1 day, 2 hours, 3 minutes</t>
+  </si>
+  <si>
+    <t>1648789K</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PWR-4330-AC       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "250W AC Power Supply for Cisco ISR 4330"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DCA210619L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ACS-4330-FANASSY  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4330 Fan Assembly"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4331 Built-In NIM controller"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NIM-1MFT-T1/E1    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "NIM-1MFT-T1/E1 - T1/E1 Serial Module"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FOC21052A61</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PVDM4-32          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "PVDM4-32 Voice DSP Module"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FOC21027LCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ISR4331-3x1GE     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Front Panel 3 ports Gigabitethernet Module"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JAB092709EL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4331 Built-In SM controller"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4331 Route Processor"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FDO20442333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Cisco ISR4331 Forwarding Processor"</t>
+  </si>
+  <si>
     <t>VG-204</t>
   </si>
   <si>
-    <t xml:space="preserve"> ISR4331/K9        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cisco ISR4331 Chassis"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> FDO2110A2MP</t>
   </si>
   <si>
-    <t>15.5(3)S4b</t>
-  </si>
-  <si>
-    <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
-  </si>
-  <si>
-    <t>23 hours, 29 minutes</t>
-  </si>
-  <si>
-    <t>1648789K</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PWR-4330-AC       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "250W AC Power Supply for Cisco ISR 4330"</t>
+    <t>1 day, 2 hours, 4 minutes</t>
   </si>
   <si>
     <t xml:space="preserve"> DCA210619LH</t>
   </si>
   <si>
-    <t xml:space="preserve"> ACS-4330-FANASSY  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cisco ISR4330 Fan Assembly"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cisco ISR4331 Built-In NIM controller"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NIM-1MFT-T1/E1    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "NIM-1MFT-T1/E1 - T1/E1 Serial Module"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> FOC210529Z3</t>
   </si>
   <si>
-    <t xml:space="preserve"> PVDM4-32          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "PVDM4-32 Voice DSP Module"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> FOC21027LLU</t>
   </si>
   <si>
-    <t xml:space="preserve"> ISR4331-3x1GE     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Front Panel 3 ports Gigabitethernet Module"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JAB092709EL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cisco ISR4331 Built-In SM controller"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cisco ISR4331 Route Processor"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> FDO204620WX</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Cisco ISR4331 Forwarding Processor"</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
@@ -164,10 +185,16 @@
     <t>recomendation</t>
   </si>
   <si>
-    <t>3%/0%</t>
+    <t>5%/0%</t>
   </si>
   <si>
     <t>1%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>2%/0%</t>
   </si>
   <si>
     <t>Variable</t>
@@ -548,7 +575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,6 +734,131 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -721,7 +873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,14 +884,14 @@
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
@@ -750,31 +902,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -785,10 +937,10 @@
         <v>1688360784</v>
       </c>
       <c r="C3" t="n">
-        <v>405609916</v>
+        <v>405687472</v>
       </c>
       <c r="D3" t="n">
-        <v>1282750868</v>
+        <v>1282673312</v>
       </c>
       <c r="E3">
         <f>IF(ISERROR(C3/B3),0,(C3/B3)*100)</f>
@@ -799,16 +951,51 @@
         <v/>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="J3">
         <f>IF((VALUE(I3)*100)&lt;=40,"Excellent",IF((VALUE(I3)*100)&lt;=60,"Good",IF((VALUE(I3)*100)&lt;=80,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1688360784</v>
+      </c>
+      <c r="C4" t="n">
+        <v>405610296</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1282750488</v>
+      </c>
+      <c r="E4">
+        <f>IF(ISERROR(C4/B4),0,(C4/B4)*100)</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>IF(E4&lt;=40,"Excellent",IF(E4&lt;=60,"Good",IF(E4&lt;=80,"Fair","Poor")))</f>
+        <v/>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4">
+        <f>IF((VALUE(I4)*100)&lt;=40,"Excellent",IF((VALUE(I4)*100)&lt;=60,"Good",IF((VALUE(I4)*100)&lt;=80,"Fair","Poor")))</f>
         <v/>
       </c>
     </row>
@@ -828,7 +1015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -841,22 +1028,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -864,10 +1051,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C2" t="n">
-        <v>357556</v>
+        <v>394621</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -887,10 +1074,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C3" t="n">
-        <v>348792</v>
+        <v>380750</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -910,13 +1097,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C4" t="n">
-        <v>78291</v>
+        <v>86488</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f>C4+D4</f>
@@ -933,10 +1120,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C5" t="n">
-        <v>50819</v>
+        <v>56381</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
@@ -956,7 +1143,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
@@ -979,7 +1166,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -997,6 +1184,147 @@
       </c>
       <c r="G7">
         <f>IF(F7&lt;=5,"Excellent",IF(F7&lt;=10,"Good",IF(F7&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="n">
+        <v>400329</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>C8+D8</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>IF(ISERROR(D8/E8),0,(D8/E8)*100)</f>
+        <v/>
+      </c>
+      <c r="G8">
+        <f>IF(F8&lt;=5,"Excellent",IF(F8&lt;=10,"Good",IF(F8&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="n">
+        <v>388084</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>C9+D9</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>IF(ISERROR(D9/E9),0,(D9/E9)*100)</f>
+        <v/>
+      </c>
+      <c r="G9">
+        <f>IF(F9&lt;=5,"Excellent",IF(F9&lt;=10,"Good",IF(F9&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="n">
+        <v>86671</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f>C10+D10</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>IF(ISERROR(D10/E10),0,(D10/E10)*100)</f>
+        <v/>
+      </c>
+      <c r="G10">
+        <f>IF(F10&lt;=5,"Excellent",IF(F10&lt;=10,"Good",IF(F10&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="n">
+        <v>56405</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f>C11+D11</f>
+        <v/>
+      </c>
+      <c r="F11">
+        <f>IF(ISERROR(D11/E11),0,(D11/E11)*100)</f>
+        <v/>
+      </c>
+      <c r="G11">
+        <f>IF(F11&lt;=5,"Excellent",IF(F11&lt;=10,"Good",IF(F11&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>C12+D12</f>
+        <v/>
+      </c>
+      <c r="F12">
+        <f>IF(ISERROR(D12/E12),0,(D12/E12)*100)</f>
+        <v/>
+      </c>
+      <c r="G12">
+        <f>IF(F12&lt;=5,"Excellent",IF(F12&lt;=10,"Good",IF(F12&lt;=20,"Fair","Poor")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>C13+D13</f>
+        <v/>
+      </c>
+      <c r="F13">
+        <f>IF(ISERROR(D13/E13),0,(D13/E13)*100)</f>
+        <v/>
+      </c>
+      <c r="G13">
+        <f>IF(F13&lt;=5,"Excellent",IF(F13&lt;=10,"Good",IF(F13&lt;=20,"Fair","Poor")))</f>
         <v/>
       </c>
     </row>
@@ -1021,22 +1349,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>